<commit_message>
added data for all categories
</commit_message>
<xml_diff>
--- a/Backend/Data/2025_First_CSEMockExamQuestionsData.xlsx
+++ b/Backend/Data/2025_First_CSEMockExamQuestionsData.xlsx
@@ -5,10 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="category_name" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Verbal" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Analytical" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Numerical" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Clerical" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="General" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t xml:space="preserve">questions</t>
   </si>
@@ -41,6 +45,207 @@
   </si>
   <si>
     <t xml:space="preserve">paragraph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which word is an antonym of "ENORMOUS"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify the misspelled word.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Committee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beginning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seperate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on the text, what is the primary goal?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading Comp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recruitment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sustainability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The organization has shifted its focus from short-term gains to long-term environmental sustainability by 2030...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 4, 9, 16, __</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finger is to Hand as Leaf is to __</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analogy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who is the tallest among the four?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo is taller than John. John is taller than Mark. Mark and Kevin are the same height.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the value of $5!$ (5 factorial)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arithmetic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solve for $y$: $2y + 10 = 30$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algebra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average of 10, 20, 30, and 40?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort: Garcia, Galsim, Galang, Gaddi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphabetizing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaddi, Galang, Garcia, Galsim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaddi, Galsim, Galang, Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galang, Gaddi, Galsim, Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaddi, Galang, Galsim, Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which pair is NOT identical?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5501-X : 5501-X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-123 : ABC-123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">998-00 : 998-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1024-B : 1024-V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A document marked "URGENT" should be:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office Proc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filed away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shredded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processed first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When was the current PH Constitution ratified?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the minimum age to be a Senator?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the national flower of the Philippines?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Symbols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gumamela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daisy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampaguita</t>
   </si>
 </sst>
 </file>
@@ -55,6 +260,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,9 +320,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -242,35 +452,98 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -282,4 +555,435 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1935</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1973</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>1945</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edit data from xlsx
</commit_message>
<xml_diff>
--- a/Backend/Data/2025_First_CSEMockExamQuestionsData.xlsx
+++ b/Backend/Data/2025_First_CSEMockExamQuestionsData.xlsx
@@ -325,7 +325,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,7 +455,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G2:G4"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G4"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G2:G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -782,7 +782,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G2:G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,7 +889,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G2:G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>